<commit_message>
Update 'Presion_vapor_entrada' minimum range, adjust the real data path in the environment configuration, and refresh pipeline results.
</commit_message>
<xml_diff>
--- a/output/resultados_pipeline.xlsx
+++ b/output/resultados_pipeline.xlsx
@@ -471,14 +471,14 @@
         <v>272.11</v>
       </c>
       <c r="D2" t="n">
-        <v>-5</v>
+        <v>263.56</v>
       </c>
       <c r="E2" t="n">
-        <v>275</v>
+        <v>272.11</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>⚠️ Fuera de rango (Ambos extremos)</t>
+          <t>OK: Dentro de rango</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -500,14 +500,14 @@
         <v>788.41</v>
       </c>
       <c r="D3" t="n">
-        <v>775</v>
+        <v>774.38</v>
       </c>
       <c r="E3" t="n">
-        <v>785</v>
+        <v>788.41</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>✅ Dentro de rango</t>
+          <t>OK: Dentro de rango</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -528,24 +528,20 @@
       <c r="C4" t="n">
         <v>403.35</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D4" t="n">
+        <v>401.19</v>
+      </c>
+      <c r="E4" t="n">
+        <v>403.35</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Sin datos de muestra</t>
+          <t>OK: Dentro de rango</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Cálculo pendiente (Métrica de severidad)</t>
         </is>
       </c>
     </row>
@@ -561,24 +557,20 @@
       <c r="C5" t="n">
         <v>538.88</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D5" t="n">
+        <v>535.14</v>
+      </c>
+      <c r="E5" t="n">
+        <v>538.88</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Sin datos de muestra</t>
+          <t>OK: Dentro de rango</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Cálculo pendiente (Métrica de severidad)</t>
         </is>
       </c>
     </row>
@@ -594,24 +586,20 @@
       <c r="C6" t="n">
         <v>174.16</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D6" t="n">
+        <v>171.45</v>
+      </c>
+      <c r="E6" t="n">
+        <v>174.16</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Sin datos de muestra</t>
+          <t>OK: Dentro de rango</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Cálculo pendiente (Métrica de severidad)</t>
         </is>
       </c>
     </row>
@@ -627,24 +615,20 @@
       <c r="C7" t="n">
         <v>166.8</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D7" t="n">
+        <v>164.26</v>
+      </c>
+      <c r="E7" t="n">
+        <v>166.8</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Sin datos de muestra</t>
+          <t>BAJO: Bajo el minimo esperado</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Cálculo pendiente (Métrica de severidad)</t>
         </is>
       </c>
     </row>
@@ -660,24 +644,20 @@
       <c r="C8" t="n">
         <v>30.38</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D8" t="n">
+        <v>29.51</v>
+      </c>
+      <c r="E8" t="n">
+        <v>30.38</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Sin datos de muestra</t>
+          <t>OK: Dentro de rango</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Cálculo pendiente (Métrica de severidad)</t>
         </is>
       </c>
     </row>

</xml_diff>